<commit_message>
edits to extraction and standardization code for infra, start filling in assumptions file
</commit_message>
<xml_diff>
--- a/data/Vulnerability/S1_Assumptions_Test.xlsx
+++ b/data/Vulnerability/S1_Assumptions_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gmhcira\data\Vulnerability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1263C1CE-DD77-406C-88A1-9F7F981E0E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCBF147-92B9-449A-A788-E974A86635A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="95">
   <si>
     <t>Hazard(s)</t>
   </si>
@@ -261,10 +261,58 @@
     <t>Infrastructure type</t>
   </si>
   <si>
-    <t>['F7.1']</t>
-  </si>
-  <si>
-    <t>[63]</t>
+    <t>Check storyline paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A restricted access major divided highway, normally with 2 or more running lanes plus emergency hard shoulder. </t>
+  </si>
+  <si>
+    <t>The most important roads in a country's system that aren't motorways.</t>
+  </si>
+  <si>
+    <t>The next most important roads in a country's system, often linking larger towns.</t>
+  </si>
+  <si>
+    <t>The next most important roads in a country's system, often linking towns.</t>
+  </si>
+  <si>
+    <t>The next most important roads in a country's system, often linking smaller towns and villages.</t>
+  </si>
+  <si>
+    <t>['F7.4', 'F7.5', 'F7.6', 'F7.7']</t>
+  </si>
+  <si>
+    <t>[F7.8, F7.9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow velocity. Abudance of sophisticated accessories. </t>
+  </si>
+  <si>
+    <t>There are more road curves. Include them as well?</t>
+  </si>
+  <si>
+    <t>[72]</t>
+  </si>
+  <si>
+    <t>[70, 75]</t>
+  </si>
+  <si>
+    <t>[69, 81]</t>
+  </si>
+  <si>
+    <t>[68, 74, 82, 89, 90]</t>
+  </si>
+  <si>
+    <t>[71, 76, 88]</t>
+  </si>
+  <si>
+    <t>Fragility functions (Flow velocity. Abudance of sophisticated accessories.) and construction costs</t>
+  </si>
+  <si>
+    <t>[73, 77, 83]</t>
+  </si>
+  <si>
+    <t>Fragility functions (Flow velocity).</t>
   </si>
 </sst>
 </file>
@@ -662,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,117 +783,143 @@
       <c r="H3" s="1"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="H4" s="5"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J4" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>77</v>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="4"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>77</v>
+      <c r="C7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="4"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>77</v>
+      <c r="C8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="4"/>
@@ -858,10 +932,12 @@
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -878,7 +954,9 @@
       <c r="C11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -895,7 +973,9 @@
       <c r="C12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1198,15 +1278,10 @@
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C11" r:id="rId8" display="\\" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C11" r:id="rId3" display="\\" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
work on assumption file, specify vuln curves and asset values per infra type
</commit_message>
<xml_diff>
--- a/data/Vulnerability/S1_Assumptions_Test.xlsx
+++ b/data/Vulnerability/S1_Assumptions_Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gmhcira\data\Vulnerability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCBF147-92B9-449A-A788-E974A86635A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8874AEB-9884-41B6-B5FB-2BE06BA9D416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flooding assumptions" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,28 @@
     <sheet name="Cyclone assumptions" sheetId="7" r:id="rId3"/>
     <sheet name="Landslide assumptions" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="118">
   <si>
     <t>Hazard(s)</t>
   </si>
@@ -165,9 +176,6 @@
     <t>Facility used to treat wastewater</t>
   </si>
   <si>
-    <t>Includes OSM tags rail, subway, tram, construction, funicular, light_rail, narrow_gauge --&gt; consider to decatogerize them??</t>
-  </si>
-  <si>
     <t>Motorway</t>
   </si>
   <si>
@@ -228,9 +236,6 @@
     <t>Vulnerability ID number</t>
   </si>
   <si>
-    <t>["","",""]</t>
-  </si>
-  <si>
     <t>Maximum damage ID number</t>
   </si>
   <si>
@@ -261,9 +266,6 @@
     <t>Infrastructure type</t>
   </si>
   <si>
-    <t>Check storyline paper</t>
-  </si>
-  <si>
     <t xml:space="preserve">A restricted access major divided highway, normally with 2 or more running lanes plus emergency hard shoulder. </t>
   </si>
   <si>
@@ -282,15 +284,6 @@
     <t>['F7.4', 'F7.5', 'F7.6', 'F7.7']</t>
   </si>
   <si>
-    <t>[F7.8, F7.9]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flow velocity. Abudance of sophisticated accessories. </t>
-  </si>
-  <si>
-    <t>There are more road curves. Include them as well?</t>
-  </si>
-  <si>
     <t>[72]</t>
   </si>
   <si>
@@ -306,20 +299,119 @@
     <t>[71, 76, 88]</t>
   </si>
   <si>
-    <t>Fragility functions (Flow velocity. Abudance of sophisticated accessories.) and construction costs</t>
-  </si>
-  <si>
     <t>[73, 77, 83]</t>
   </si>
   <si>
-    <t>Fragility functions (Flow velocity).</t>
+    <t xml:space="preserve">There are more road curves, selected only the van Ginkel curves. Include the others as well? Also, how to deal with the various cost estimates. Write code to select all the cost estimates, provide a range and do calculations for minimum, maximum and median/mean?  </t>
+  </si>
+  <si>
+    <t>Full sized passenger or freight train tracks in the standard gauge for the country or state.</t>
+  </si>
+  <si>
+    <t>['F8.1', 'F8.2', 'F8.3', 'F8.4', 'F8.5', 'F8.6', 'F8.6a', 'F8.6b', 'F8.7']</t>
+  </si>
+  <si>
+    <t>[46, 49, 50, 51, 52, 53, 54, 55, 56, 57, 61, 62, 78]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also include F8.6a F8.6b? We don't have lower and upper boundaries of other curves? Asset value is highly dependent on whether the rail is electrified or not. Use this kind of additional information for analysis and discuss ways to code it? Note: for the Netherlands for example, only for 51% information is provided on electrification of the railways. Use specific (non-)electrification values for known assets and treat it as an unknown for the others? OR make assumptions about electrification of railway? </t>
+  </si>
+  <si>
+    <t>Remaining type of roads, such as residential streets where pedestrians have legal priority over cars, speeds are kept very low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a vulnerability curve for airports is provided by Kok et al. (2005). They also provide a maximum damage value given in damage per exposed footprint of an airport (euro/m2). The usage of this in combination with the spatial airport data, which are extracted from OSM in polygon format, may lead to an overestimation of the direct damages to airports. These polygons represent the airports as a whole, including areas that are covered by structural components, but also areas that are less important for risk analysis (e.g., grass). We therefore decide to break down the direct damages to airports by presenting structural damages to terminals and runways.  For terminals, we use the vulnerability curve of Kok et al. (2005) in combination with maximum damage based on construction costs estimated by Carruthers (2013). Due to absence of more specific vulnerability curves for runways, we apply the vulnerability curve of Huizinga et al. (2017) estimated for roads. The maximum damages are based on construction costs for runway types made of concrete and asphalt (Gibson et al., 2011). </t>
+  </si>
+  <si>
+    <t>['F7.8', 'F7.9']</t>
+  </si>
+  <si>
+    <t>['F9.1','F9.2', 'F9.3']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3]</t>
+  </si>
+  <si>
+    <t>Maximum damages range between 98-114 euros/m2. Do we (also) want to calculate the damage on airport polygon data?</t>
+  </si>
+  <si>
+    <t>Add Carruthers (2013) data to database</t>
+  </si>
+  <si>
+    <t>Fragility functions and asset values</t>
+  </si>
+  <si>
+    <t>Fragility functions (Flow velocity. Abudance of sophisticated accessories.) and asset values</t>
+  </si>
+  <si>
+    <t>Fragility functions (Flow velocity) and asset values</t>
+  </si>
+  <si>
+    <t>Fragility functions (Flow velocity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do we want to calculate airport damages? Based on aerodrome polygon or specific assets within aerodrome? Now using terminal and runway, but can also add other aerodrome assets as well? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Towers with greater heigts (could be above 100m) for transmitting radio applications like television, radio, mobile phone or officials radio. It is often made from concrete and usually a visible landmark. </t>
+  </si>
+  <si>
+    <t>['F10.1']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We assume that masts are more vulnerable to flooding as they are smaller structures compared to communication towers. We therefore apply the vulnerability curve proposed by Kok et al. (2015) for electricity and communication systems, which assumes higher damage factors compared to the function used for communication towers. The maximum damage of masts is based on construction costs provided by Foster (2015) and Liebman (2018). </t>
+  </si>
+  <si>
+    <t>Add Foster (2015) and Liebman (2018) data to database</t>
+  </si>
+  <si>
+    <t>Copy paste power tower curve here</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We use the vulnerability curve of FEMA (2013) that we also apply for large power towers for communication towers, because of similar structural characteristics. We assume that only little damage occurs to large communication towers, and this is what this vulnerability curve embodies. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">We use this in combination with maximum damages for 'other community facility' provided by FEMA (2013) as no specific construction cost data were available for communication towers. </t>
+    </r>
+  </si>
+  <si>
+    <t>If multiple curves, then vulnerability curves. Otherwise, -25% and +25% or asset value</t>
+  </si>
+  <si>
+    <t>Asset values</t>
+  </si>
+  <si>
+    <t>['F21.6', 'F21.8', 'F21.9', 'F21.12']</t>
+  </si>
+  <si>
+    <t>['F21.6', 'F21.7', 'F21.8', 'F21.10', 'F21.11', 'F21.13']</t>
+  </si>
+  <si>
+    <t>[8, 9, 11*, 91, 92]</t>
+  </si>
+  <si>
+    <t>[11*, 12, 13, 14]</t>
+  </si>
+  <si>
+    <t>Include Huizinga max. damages per country?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +443,21 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -391,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -428,6 +535,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +823,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -726,7 +838,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -741,22 +853,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>2</v>
@@ -766,65 +878,73 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>45</v>
+      <c r="C3" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H4" s="5"/>
       <c r="J4" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="H5" s="5"/>
       <c r="J5" s="3"/>
@@ -834,19 +954,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -858,19 +978,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -882,105 +1002,130 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="4"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="319" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s">
+        <v>99</v>
+      </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="319" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="H11" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="319" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -1010,8 +1155,6 @@
       <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1108,7 +1251,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
@@ -1116,16 +1259,24 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+        <v>104</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
@@ -1133,13 +1284,21 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>112</v>
+      </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1204,20 +1363,20 @@
         <v>30</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H26" s="9"/>
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>52</v>
+      <c r="C27" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="H27" s="5"/>
       <c r="J27" s="8"/>
@@ -1249,11 +1408,19 @@
       <c r="C29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G29" s="4"/>
-      <c r="J29" s="6"/>
+      <c r="J29" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
@@ -1265,20 +1432,28 @@
       <c r="C30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G30" s="4"/>
-      <c r="J30" s="6"/>
+      <c r="J30" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C11" r:id="rId3" display="\\" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C9" r:id="rId1" display="\\" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C11" r:id="rId2" display="\\" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId3" display="\\" xr:uid="{1E3AFFB4-656F-459B-9194-FB3F0C197691}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1306,7 +1481,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1327,16 +1502,16 @@
         <v>6</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>2</v>
@@ -1344,7 +1519,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1359,13 +1534,13 @@
     </row>
     <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1374,13 +1549,13 @@
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1389,13 +1564,13 @@
     </row>
     <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1405,13 +1580,13 @@
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1421,13 +1596,13 @@
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1437,10 +1612,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
@@ -1453,7 +1628,7 @@
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>16</v>
@@ -1468,13 +1643,13 @@
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1483,13 +1658,13 @@
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1498,7 +1673,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
@@ -1514,7 +1689,7 @@
     </row>
     <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>25</v>
@@ -1530,7 +1705,7 @@
     </row>
     <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>26</v>
@@ -1546,7 +1721,7 @@
     </row>
     <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
@@ -1561,7 +1736,7 @@
     </row>
     <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -1577,7 +1752,7 @@
     </row>
     <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>19</v>
@@ -1593,7 +1768,7 @@
     </row>
     <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>20</v>
@@ -1609,13 +1784,13 @@
     </row>
     <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
@@ -1624,13 +1799,13 @@
     </row>
     <row r="21" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
@@ -1639,7 +1814,7 @@
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>21</v>
@@ -1653,7 +1828,7 @@
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>22</v>
@@ -1667,7 +1842,7 @@
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>23</v>
@@ -1682,7 +1857,7 @@
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>24</v>
@@ -1696,33 +1871,33 @@
     </row>
     <row r="26" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="5"/>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="5"/>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>11</v>
@@ -1737,7 +1912,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>33</v>
@@ -1751,7 +1926,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>34</v>
@@ -1804,7 +1979,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1825,16 +2000,16 @@
         <v>6</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>2</v>
@@ -1846,7 +2021,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1861,13 +2036,13 @@
     </row>
     <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1876,13 +2051,13 @@
     </row>
     <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1891,13 +2066,13 @@
     </row>
     <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1907,13 +2082,13 @@
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1923,13 +2098,13 @@
     </row>
     <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1939,10 +2114,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
@@ -1955,7 +2130,7 @@
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>16</v>
@@ -1970,13 +2145,13 @@
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1985,13 +2160,13 @@
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2000,7 +2175,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
@@ -2016,7 +2191,7 @@
     </row>
     <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>25</v>
@@ -2033,7 +2208,7 @@
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>26</v>
@@ -2050,7 +2225,7 @@
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
@@ -2065,7 +2240,7 @@
     </row>
     <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -2081,7 +2256,7 @@
     </row>
     <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>19</v>
@@ -2098,7 +2273,7 @@
     </row>
     <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>20</v>
@@ -2115,13 +2290,13 @@
     </row>
     <row r="20" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
@@ -2130,13 +2305,13 @@
     </row>
     <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
@@ -2145,7 +2320,7 @@
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>21</v>
@@ -2159,7 +2334,7 @@
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>22</v>
@@ -2173,7 +2348,7 @@
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>23</v>
@@ -2188,7 +2363,7 @@
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>24</v>
@@ -2203,33 +2378,33 @@
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="5"/>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="5"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>11</v>
@@ -2244,7 +2419,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>33</v>
@@ -2258,7 +2433,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>34</v>
@@ -2310,7 +2485,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2331,16 +2506,16 @@
         <v>6</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>2</v>
@@ -2352,7 +2527,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -2367,13 +2542,13 @@
     </row>
     <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2382,13 +2557,13 @@
     </row>
     <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2397,13 +2572,13 @@
     </row>
     <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -2413,13 +2588,13 @@
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -2429,13 +2604,13 @@
     </row>
     <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -2445,10 +2620,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
@@ -2461,7 +2636,7 @@
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>16</v>
@@ -2476,13 +2651,13 @@
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -2491,13 +2666,13 @@
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2506,7 +2681,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
@@ -2522,7 +2697,7 @@
     </row>
     <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>25</v>
@@ -2539,7 +2714,7 @@
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>26</v>
@@ -2556,7 +2731,7 @@
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
@@ -2571,7 +2746,7 @@
     </row>
     <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -2587,7 +2762,7 @@
     </row>
     <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>19</v>
@@ -2604,7 +2779,7 @@
     </row>
     <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>20</v>
@@ -2621,13 +2796,13 @@
     </row>
     <row r="20" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
@@ -2636,13 +2811,13 @@
     </row>
     <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
@@ -2651,7 +2826,7 @@
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>21</v>
@@ -2665,7 +2840,7 @@
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>22</v>
@@ -2679,7 +2854,7 @@
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>23</v>
@@ -2694,7 +2869,7 @@
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>24</v>
@@ -2709,33 +2884,33 @@
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="5"/>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="5"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>11</v>
@@ -2750,7 +2925,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>33</v>
@@ -2764,7 +2939,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
first complete version assumption file, specify vuln curves and asset values per infra type
</commit_message>
<xml_diff>
--- a/data/Vulnerability/S1_Assumptions_Test.xlsx
+++ b/data/Vulnerability/S1_Assumptions_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gmhcira\data\Vulnerability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8874AEB-9884-41B6-B5FB-2BE06BA9D416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6625B5F9-D3FF-4883-A191-4B3748B78212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flooding assumptions" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="172">
   <si>
     <t>Hazard(s)</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Add Foster (2015) and Liebman (2018) data to database</t>
-  </si>
-  <si>
-    <t>Copy paste power tower curve here</t>
   </si>
   <si>
     <t>[5]</t>
@@ -406,12 +403,213 @@
   <si>
     <t>Include Huizinga max. damages per country?</t>
   </si>
+  <si>
+    <t>Clinic</t>
+  </si>
+  <si>
+    <t>Doctors</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Dentist</t>
+  </si>
+  <si>
+    <t>Pharmacy</t>
+  </si>
+  <si>
+    <t>Physiotherapist</t>
+  </si>
+  <si>
+    <t>Alternative</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>Optometrist</t>
+  </si>
+  <si>
+    <t>Rehabilitation</t>
+  </si>
+  <si>
+    <t>Blood donation</t>
+  </si>
+  <si>
+    <t>Birthing center</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>Kindergarten</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>['F1.1', 'F1.2', 'F1.3', 'F1.4', 'F1.5', 'F1.6', 'F1.7']</t>
+  </si>
+  <si>
+    <t>[4, 10, 23, 28, 29, 30, 113-179]</t>
+  </si>
+  <si>
+    <t>Indicate tye of power plant? Use tag: plant:source for this, needs to be added to OSM flex in case we're interested in further specifying this. Also, add code that certain vulnerability curves can only be used with certain asset values? E.g., wind turbine curve can only be combined with asset value for wind turbines? Or we can just stick with the general curves and asset values (of FEMA)</t>
+  </si>
+  <si>
+    <t>Fragility functions (capacity and power plant type) and asset value (capacity and power plant type)</t>
+  </si>
+  <si>
+    <t>['F2.1', 'F2.2', 'F2.3']</t>
+  </si>
+  <si>
+    <t>[94, 95, 96, 97]</t>
+  </si>
+  <si>
+    <t>Fragility functions and asset value (capacity-based)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the power towers and power poles we apply the vulnerability curve for T&amp;D systems. Again, maximum damages were not provided and we therefore use construction costs for power towers and poles. Midcontinent Interdependent System Operator (MISO) provides yearly reports with estimated costs for various energy assets, including power towers and poles. OSM describes power towers as assets that carry high-voltage overhead power lines, and are often constructed from steel, while power poles are often made from wood. For this reason, we use the construction costs for single- and double circuit steel towers built for a range of high-voltage overhead lines for determining the maximum damage for power towers, while we only use construction costs for wooden poles (single and double circuit) for determining the maximum damage for power poles.   </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[34] </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ MISO</t>
+    </r>
+  </si>
+  <si>
+    <t>Fragility functions and asset value (design-based)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[31, 32, 33] </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ MISO</t>
+    </r>
+  </si>
+  <si>
+    <t>['F5.1']</t>
+  </si>
+  <si>
+    <t>['F6.1', 'F6.2']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We conduct the construction costs for underground cables from Hall (2009). Based on a survey conducted by Burns &amp; McDonnell (n.d.), underground cables are not likely to suffer direct damage due to flooding. Flooding impacts the above grade equipment that the cables are connected with, and this failure may propagate into the whole energy circuit. This finding is also supported by Hall (2009). However, uprooting of trees (Hall, 2009) and soil liquefaction (Miyamoto, 2019) may cause damages to underground infrastructure. For this study, we assume that no damage occurs to underground cables due to flooding as we assume a relative low flow velocity.  </t>
+  </si>
+  <si>
+    <t>add Hall (2009) data to database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We therefore base our maximum damages on construction costs for overhead lines in urban (for lines) and rural (for minor lines) areas provided by Hall (2009). </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[24, 25, 26, 27, 36, 37, 38, 39] </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ Hall (2009)</t>
+    </r>
+  </si>
+  <si>
+    <t>Asset values (construction material?)</t>
+  </si>
+  <si>
+    <t>Reclassify to line? Or adjust asset values (e.g., use construction costs for transmission lines carried on wooden poles for minor lines and construction costs for better quality materials for lines)</t>
+  </si>
+  <si>
+    <t>['F18.1', 'F18.2', 'F18.3', 'F18.4', 'F18.5', 'F18.6']</t>
+  </si>
+  <si>
+    <t>[102, 103]</t>
+  </si>
+  <si>
+    <t>Fragility functions (capacity-based and design standards) and asset values</t>
+  </si>
+  <si>
+    <t>['F15.1']</t>
+  </si>
+  <si>
+    <t>[112]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset value </t>
+  </si>
+  <si>
+    <t>[-25% - +25%]</t>
+  </si>
+  <si>
+    <t>['F13.4']</t>
+  </si>
+  <si>
+    <t>['F13.1', 'F13.2', 'F13.3', 'F13.5']</t>
+  </si>
+  <si>
+    <t>Water storage tank</t>
+  </si>
+  <si>
+    <t>Storage tanks are containers that hold drinking water, used for short- or long-term storage</t>
+  </si>
+  <si>
+    <t>[107]</t>
+  </si>
+  <si>
+    <t>[104, 105, 106, 108]</t>
+  </si>
+  <si>
+    <t>['F13.1', 'F13.2', 'F13.3', 'F13.4', 'F13.5']</t>
+  </si>
+  <si>
+    <t>[104, 105, 106, 107, 108]</t>
+  </si>
+  <si>
+    <t>Fragility functions (construction material, storage tank height) and asset values (construction material, storage tank height)</t>
+  </si>
+  <si>
+    <t>['F14.1', 'F14.2', 'F14.3', 'F14.4', 'F14.5', 'F14.6', 'F14.7', 'F14.8', 'F14.9', 'F14.10']</t>
+  </si>
+  <si>
+    <t>[109, 110, 111]</t>
+  </si>
+  <si>
+    <t>Fragility functions (capacity and design type) and asset value (capacity-based)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,9 +653,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -495,10 +700,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -522,9 +728,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -532,16 +735,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -820,42 +1040,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.81640625" style="1" customWidth="1"/>
-    <col min="4" max="7" width="25.7265625" customWidth="1"/>
-    <col min="8" max="8" width="45" customWidth="1"/>
-    <col min="10" max="10" width="100.26953125" style="2" customWidth="1"/>
+    <col min="4" max="7" width="25.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="1"/>
+    <col min="10" max="10" width="100.26953125" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" s="22" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="12" t="s">
@@ -873,41 +1095,39 @@
       <c r="H2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -923,15 +1143,15 @@
         <v>100</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -947,19 +1167,18 @@
         <v>100</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -970,20 +1189,19 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="8"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -994,20 +1212,19 @@
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="8"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1018,20 +1235,19 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="8"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1042,57 +1258,55 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="319" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>99</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="319" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:10" s="5" customFormat="1" ht="319" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>95</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
         <v>93</v>
       </c>
@@ -1100,11 +1314,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="319" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:10" s="5" customFormat="1" ht="319" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1113,13 +1327,12 @@
       <c r="D12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="16" t="s">
         <v>98</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
         <v>93</v>
       </c>
@@ -1127,323 +1340,729 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="D13" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>151</v>
+      </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="H13" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="D14" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="H14" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="D15" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="H15" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="D16" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="8" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="D17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>140</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" ht="261" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="D18" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="H18" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="261" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="D19" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="8"/>
+      <c r="H19" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="145" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>111</v>
+      <c r="F20" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J20" s="6"/>
+        <v>109</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="145" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>112</v>
+      <c r="F21" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    </row>
+    <row r="22" spans="1:10" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:10" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="4" t="s">
+    <row r="24" spans="1:10" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>168</v>
+      </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="25" spans="1:10" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="10" t="s">
+      <c r="D26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="10" t="s">
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="5"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="J30" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="E42" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="J29" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="4" t="s">
+    </row>
+    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="4" t="s">
+      <c r="F43" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="J30" s="4" t="s">
-        <v>117</v>
+    </row>
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1454,9 +2073,12 @@
     <hyperlink ref="C9" r:id="rId1" display="\\" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C11" r:id="rId2" display="\\" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="C10" r:id="rId3" display="\\" xr:uid="{1E3AFFB4-656F-459B-9194-FB3F0C197691}"/>
+    <hyperlink ref="C30" r:id="rId4" xr:uid="{4CC1A6A9-4232-45F0-9201-EC8F28D3C30E}"/>
+    <hyperlink ref="C31:C45" r:id="rId5" display="\\" xr:uid="{433B81EC-3149-4D3F-B6E1-418BFF9CE36B}"/>
+    <hyperlink ref="C46" r:id="rId6" xr:uid="{35829217-814D-485A-9071-E3F41459068B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1491,29 +2113,29 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:8" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:8" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1989,33 +2611,33 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:10" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2495,33 +3117,33 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:10" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="14" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OSM-flex adjustments and improved workflow datatypes
</commit_message>
<xml_diff>
--- a/data/Vulnerability/S1_Assumptions_Test.xlsx
+++ b/data/Vulnerability/S1_Assumptions_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gmhcira\data\Vulnerability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6625B5F9-D3FF-4883-A191-4B3748B78212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B158D5C1-E966-488A-99B8-D09DA1BFB515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="176">
   <si>
     <t>Hazard(s)</t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t>['F8.1', 'F8.2', 'F8.3', 'F8.4', 'F8.5', 'F8.6', 'F8.6a', 'F8.6b', 'F8.7']</t>
-  </si>
-  <si>
-    <t>[46, 49, 50, 51, 52, 53, 54, 55, 56, 57, 61, 62, 78]</t>
   </si>
   <si>
     <t xml:space="preserve">Also include F8.6a F8.6b? We don't have lower and upper boundaries of other curves? Asset value is highly dependent on whether the rail is electrified or not. Use this kind of additional information for analysis and discuss ways to code it? Note: for the Netherlands for example, only for 51% information is provided on electrification of the railways. Use specific (non-)electrification values for known assets and treat it as an unknown for the others? OR make assumptions about electrification of railway? </t>
@@ -578,9 +575,6 @@
     <t>Water storage tank</t>
   </si>
   <si>
-    <t>Storage tanks are containers that hold drinking water, used for short- or long-term storage</t>
-  </si>
-  <si>
     <t>[107]</t>
   </si>
   <si>
@@ -603,6 +597,24 @@
   </si>
   <si>
     <t>Fragility functions (capacity and design type) and asset value (capacity-based)</t>
+  </si>
+  <si>
+    <t>[46, 49, 50, 51, 52, 53, 54, 55, 56, 61, 62, 78]</t>
+  </si>
+  <si>
+    <t>Include cost number 57?</t>
+  </si>
+  <si>
+    <t>Maximum damage ID number (based on original file - delete)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage tanks are containers that hold drinking water, used for short- or long-term storage. Could be overground, underground or partially underground. </t>
+  </si>
+  <si>
+    <t>Structure that contains a water tank at an altitude to pressurize the water distribution network. Equivalent to an elevated storage tank.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water works  (or water treatment plant) are structures where drinking water is found and applied to the waterpipes network. The public supply of water is stored and treated in this system of buildings and pipes. </t>
   </si>
 </sst>
 </file>
@@ -738,14 +750,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -758,6 +764,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1040,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1051,26 +1063,27 @@
     <col min="1" max="1" width="13.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.81640625" style="1" customWidth="1"/>
-    <col min="4" max="7" width="25.7265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="100.26953125" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="8" width="25.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="1"/>
+    <col min="11" max="11" width="100.26953125" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:10" s="22" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:12" s="20" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -1087,20 +1100,23 @@
         <v>65</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1114,16 +1130,22 @@
         <v>89</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="L3" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1140,14 +1162,17 @@
         <v>84</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="J4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="K4" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1164,11 +1189,14 @@
         <v>83</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1179,19 +1207,22 @@
         <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1202,19 +1233,22 @@
         <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>85</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1225,19 +1259,22 @@
         <v>79</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
@@ -1245,22 +1282,25 @@
         <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>86</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="319" x14ac:dyDescent="0.35">
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="319" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
@@ -1271,24 +1311,27 @@
         <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" ht="319" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="319" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1299,22 +1342,25 @@
         <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="5" customFormat="1" ht="319" x14ac:dyDescent="0.35">
+      <c r="F11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="5" customFormat="1" ht="319" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
@@ -1328,19 +1374,22 @@
         <v>80</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="203" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
@@ -1351,21 +1400,24 @@
         <v>14</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="F13" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1376,19 +1428,22 @@
         <v>35</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>149</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1399,22 +1454,25 @@
         <v>36</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>149</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
@@ -1425,22 +1483,25 @@
         <v>39</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="J16" s="5"/>
+      <c r="K16" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>3</v>
       </c>
@@ -1451,19 +1512,22 @@
         <v>40</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="261" x14ac:dyDescent="0.35">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" ht="261" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -1474,21 +1538,24 @@
         <v>38</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="261" x14ac:dyDescent="0.35">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" ht="261" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1499,21 +1566,24 @@
         <v>37</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+      <c r="G19" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
@@ -1521,23 +1591,26 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="145" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -1548,20 +1621,23 @@
         <v>48</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:11" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1569,23 +1645,26 @@
         <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -1596,20 +1675,23 @@
         <v>42</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
@@ -1620,38 +1702,44 @@
         <v>29</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="F25" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" s="5" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
@@ -1659,423 +1747,468 @@
         <v>24</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:10" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="9" t="s">
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" s="23" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" s="21" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>44</v>
+        <v>116</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="H29" s="5"/>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="K29" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="J30" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>112</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="F42" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="F43" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="F44" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="F45" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>99</v>
+      <c r="G45" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C9" r:id="rId1" display="\\" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C11" r:id="rId2" display="\\" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="C10" r:id="rId3" display="\\" xr:uid="{1E3AFFB4-656F-459B-9194-FB3F0C197691}"/>
-    <hyperlink ref="C30" r:id="rId4" xr:uid="{4CC1A6A9-4232-45F0-9201-EC8F28D3C30E}"/>
-    <hyperlink ref="C31:C45" r:id="rId5" display="\\" xr:uid="{433B81EC-3149-4D3F-B6E1-418BFF9CE36B}"/>
-    <hyperlink ref="C46" r:id="rId6" xr:uid="{35829217-814D-485A-9071-E3F41459068B}"/>
+    <hyperlink ref="C29" r:id="rId4" xr:uid="{4CC1A6A9-4232-45F0-9201-EC8F28D3C30E}"/>
+    <hyperlink ref="C30:C44" r:id="rId5" display="\\" xr:uid="{433B81EC-3149-4D3F-B6E1-418BFF9CE36B}"/>
+    <hyperlink ref="C45" r:id="rId6" xr:uid="{35829217-814D-485A-9071-E3F41459068B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -2102,16 +2235,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
@@ -2600,16 +2733,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
@@ -3106,16 +3239,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">

</xml_diff>